<commit_message>
updated R-git commands list
</commit_message>
<xml_diff>
--- a/_r-rstudio-update-steps-refs.xlsx
+++ b/_r-rstudio-update-steps-refs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Winston\Documents\_MyStuff\7_projects\tech-sandbox\24-r-updates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31EC57F8-C96A-4D3A-BBA1-26B65D0A9F9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9977843-1EC7-45A6-9B56-F844165CC3B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="14651" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>update rstudio</t>
   </si>
@@ -79,6 +79,24 @@
   </si>
   <si>
     <t>returns username and email as on github</t>
+  </si>
+  <si>
+    <t>add git repo to existing R project</t>
+  </si>
+  <si>
+    <t>open the R project &amp; go to console</t>
+  </si>
+  <si>
+    <t>library(usethis)</t>
+  </si>
+  <si>
+    <t>use_git()</t>
+  </si>
+  <si>
+    <t>follow the user prompts - confirm to add files to the repo</t>
+  </si>
+  <si>
+    <t>restart Rstudio &amp; look for git tab in upper right block</t>
   </si>
 </sst>
 </file>
@@ -424,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:D24"/>
+  <dimension ref="B2:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -518,6 +536,36 @@
       </c>
       <c r="D24" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B27" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B28" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B29" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B30" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B31" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>